<commit_message>
Classificado até o 299
</commit_message>
<xml_diff>
--- a/havaiana.xlsx
+++ b/havaiana.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilh\OneDrive - Insper - Institudo de Ensino e Pesquisa\2° Semestre\Ciência dos Dados\Projeto1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilh\OneDrive - Insper - Institudo de Ensino e Pesquisa\2° Semestre\Ciência dos Dados\Projeto1-Ciedados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="710" documentId="11_93449983DA0BA716E111B8FDCD5C049251A7D67D" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0B50228D-C972-473A-A910-E6A881891D28}"/>
+  <xr:revisionPtr revIDLastSave="749" documentId="11_93449983DA0BA716E111B8FDCD5C049251A7D67D" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6B7ED218-5F61-4BF8-B648-885ABD42A233}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3063,8 +3063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A251" workbookViewId="0">
-      <selection activeCell="B272" sqref="B272"/>
+    <sheetView tabSelected="1" topLeftCell="A266" workbookViewId="0">
+      <selection activeCell="B299" sqref="B299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5245,163 +5245,247 @@
       <c r="A272" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B272">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B273">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B274">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B275">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B276">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B277">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B278">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B279">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B280">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B281">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B282">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B283">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B284">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B285">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B286">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B287">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B288">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B289">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B290">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B291">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B292">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B293">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B294">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B295">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B296">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B297">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B298">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B299">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>303</v>
       </c>

</xml_diff>

<commit_message>
Novas classificações no Teste
</commit_message>
<xml_diff>
--- a/havaiana.xlsx
+++ b/havaiana.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tales De Bragança\Downloads\Projeto1-Ciedados-master\Projeto1-Ciedados-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilh\OneDrive - Insper - Institudo de Ensino e Pesquisa\2° Semestre\Ciência dos Dados\Projeto1-Ciedados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66035D28-82FE-4E14-9B71-4AD614A9F8D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="6_{1388BAEF-BB38-4AB5-96FF-C5BA3AC9A653}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B1E5B71F-0CE2-4E59-8703-F2191FA27B43}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="830">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="830">
   <si>
     <t>Treinamento</t>
   </si>
@@ -3063,7 +3063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B480" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B501" sqref="B501"/>
     </sheetView>
   </sheetViews>
@@ -6707,10 +6707,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A328"/>
+  <dimension ref="A1:B328"/>
   <sheetViews>
-    <sheetView topLeftCell="A294" workbookViewId="0">
-      <selection activeCell="A299" sqref="A299"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6719,562 +6719,862 @@
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>520</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>532</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>536</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>543</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>551</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>555</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>556</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>558</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>560</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>565</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>566</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>572</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>576</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>577</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>579</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>580</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>581</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>582</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>583</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>584</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B84">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>585</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>587</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B87">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>589</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B89">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>590</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>592</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B92">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>594</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>595</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>596</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>597</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>598</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B98">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>599</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>600</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>605</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>607</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>612</v>
       </c>

</xml_diff>

<commit_message>
Teste classificados até o final
</commit_message>
<xml_diff>
--- a/havaiana.xlsx
+++ b/havaiana.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilh\OneDrive - Insper - Institudo de Ensino e Pesquisa\2° Semestre\Ciência dos Dados\Projeto1-Ciedados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="6_{1388BAEF-BB38-4AB5-96FF-C5BA3AC9A653}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B1E5B71F-0CE2-4E59-8703-F2191FA27B43}"/>
+  <xr:revisionPtr revIDLastSave="116" documentId="6_{1388BAEF-BB38-4AB5-96FF-C5BA3AC9A653}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CBFC8002-02FB-4D0D-88EB-A94A3EC21982}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6709,8 +6709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B328"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A101" sqref="A101"/>
+    <sheetView tabSelected="1" topLeftCell="A303" workbookViewId="0">
+      <selection activeCell="B201" sqref="B201:B328"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7523,1140 +7523,1824 @@
       <c r="A101" t="s">
         <v>601</v>
       </c>
+      <c r="B101">
+        <v>1</v>
+      </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>602</v>
       </c>
+      <c r="B102">
+        <v>0</v>
+      </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>603</v>
       </c>
+      <c r="B103">
+        <v>2</v>
+      </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>604</v>
       </c>
+      <c r="B104">
+        <v>2</v>
+      </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>605</v>
       </c>
+      <c r="B105">
+        <v>0</v>
+      </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>606</v>
       </c>
+      <c r="B106">
+        <v>0</v>
+      </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>607</v>
       </c>
+      <c r="B107">
+        <v>2</v>
+      </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>608</v>
       </c>
+      <c r="B108">
+        <v>0</v>
+      </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>609</v>
       </c>
+      <c r="B109">
+        <v>1</v>
+      </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>610</v>
       </c>
+      <c r="B110">
+        <v>0</v>
+      </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>611</v>
       </c>
+      <c r="B111">
+        <v>1</v>
+      </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>612</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B112">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>613</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>614</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>615</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>616</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B116">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B117">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>618</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>619</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>620</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B120">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>621</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>622</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>623</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>625</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>626</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>627</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B127">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>628</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>629</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>630</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>631</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B131">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>632</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B132">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>633</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B134">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>635</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>636</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>637</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B137">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>638</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B138">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>640</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B140">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>641</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>642</v>
       </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B142">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>643</v>
       </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B143">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>644</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>645</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>646</v>
       </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>647</v>
       </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>648</v>
       </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>649</v>
       </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B149">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>650</v>
       </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>651</v>
       </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>653</v>
       </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B153">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>654</v>
       </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>655</v>
       </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>656</v>
       </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>657</v>
       </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B157">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>659</v>
       </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>660</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>661</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B161">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>662</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>663</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B163">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>664</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>665</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>666</v>
       </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B166">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>667</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>668</v>
       </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>669</v>
       </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B169">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>670</v>
       </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>671</v>
       </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>672</v>
       </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>673</v>
       </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B173">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>674</v>
       </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B174">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>675</v>
       </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B175">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>676</v>
       </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B177">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>678</v>
       </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>680</v>
       </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B180">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>681</v>
       </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B181">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>682</v>
       </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B182">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>683</v>
       </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B183">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>684</v>
       </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B184">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>685</v>
       </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B185">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>686</v>
       </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B186">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>687</v>
       </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B187">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>688</v>
       </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B188">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B189">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>690</v>
       </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>691</v>
       </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B191">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>692</v>
       </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B192">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>693</v>
       </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B193">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>694</v>
       </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B194">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>695</v>
       </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B195">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>696</v>
       </c>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B196">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>697</v>
       </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>698</v>
       </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B198">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>699</v>
       </c>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B199">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>700</v>
       </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>701</v>
       </c>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B201">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>702</v>
       </c>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B202">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>703</v>
       </c>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B203">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>704</v>
       </c>
-    </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B204">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>705</v>
       </c>
-    </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B205">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>706</v>
       </c>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B206">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>707</v>
       </c>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B207">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>708</v>
       </c>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B208">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>709</v>
       </c>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B209">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>710</v>
       </c>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B210">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>711</v>
       </c>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>712</v>
       </c>
-    </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B212">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>713</v>
       </c>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B213">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>714</v>
       </c>
-    </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B214">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>715</v>
       </c>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B215">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>716</v>
       </c>
-    </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>717</v>
       </c>
-    </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B217">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>718</v>
       </c>
-    </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B218">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>719</v>
       </c>
-    </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B219">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>720</v>
       </c>
-    </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B220">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>721</v>
       </c>
-    </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B221">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>722</v>
       </c>
-    </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B222">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>723</v>
       </c>
-    </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B223">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>724</v>
       </c>
-    </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B224">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>725</v>
       </c>
-    </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B225">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>726</v>
       </c>
-    </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B226">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>727</v>
       </c>
-    </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B227">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>728</v>
       </c>
-    </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B228">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>729</v>
       </c>
-    </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B229">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>730</v>
       </c>
-    </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B230">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>731</v>
       </c>
-    </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B231">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>732</v>
       </c>
-    </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B232">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>733</v>
       </c>
-    </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B233">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B234">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>735</v>
       </c>
-    </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B235">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>736</v>
       </c>
-    </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B236">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>737</v>
       </c>
-    </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B237">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B238">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>739</v>
       </c>
-    </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B239">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>740</v>
       </c>
-    </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B240">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>741</v>
       </c>
-    </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B241">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>742</v>
       </c>
-    </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B242">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>743</v>
       </c>
-    </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B243">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B244">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>745</v>
       </c>
-    </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B245">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>746</v>
       </c>
-    </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B246">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>747</v>
       </c>
-    </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B247">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>748</v>
       </c>
-    </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B248">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>749</v>
       </c>
-    </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B249">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>750</v>
       </c>
-    </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B250">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>751</v>
       </c>
-    </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B251">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>752</v>
       </c>
-    </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B252">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>753</v>
       </c>
-    </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B253">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>754</v>
       </c>
-    </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B254">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>755</v>
       </c>
-    </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B255">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>756</v>
       </c>
-    </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B256">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>757</v>
       </c>
-    </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B257">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>758</v>
       </c>
-    </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B258">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>759</v>
       </c>
-    </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B259">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>760</v>
       </c>
-    </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B260">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>761</v>
       </c>
-    </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B261">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>762</v>
       </c>
-    </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B262">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>763</v>
       </c>
-    </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B263">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>764</v>
       </c>
-    </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B264">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>765</v>
       </c>
-    </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B265">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>766</v>
       </c>
-    </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B266">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>767</v>
       </c>
-    </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B267">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>768</v>
       </c>
-    </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B268">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>769</v>
       </c>
-    </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B269">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>770</v>
       </c>
-    </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B270">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>771</v>
       </c>
-    </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B271">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>772</v>
       </c>
-    </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B272">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>773</v>
       </c>
-    </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B273">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>774</v>
       </c>
-    </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B274">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>775</v>
       </c>
-    </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B275">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>776</v>
       </c>
-    </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B276">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>777</v>
       </c>
-    </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B277">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>778</v>
       </c>
-    </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B278">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>779</v>
       </c>
-    </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B279">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>780</v>
       </c>
-    </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B280">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>781</v>
       </c>
-    </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B281">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>782</v>
       </c>
-    </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B282">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B283">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B284">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>785</v>
       </c>
-    </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B285">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>786</v>
       </c>
-    </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B286">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>787</v>
       </c>
-    </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B287">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>788</v>
       </c>
-    </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B288">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>789</v>
       </c>
-    </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B289">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B290">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B291">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>792</v>
       </c>
-    </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B292">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>793</v>
       </c>
-    </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B293">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>794</v>
       </c>
-    </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B294">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>795</v>
       </c>
-    </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B295">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>796</v>
       </c>
-    </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B296">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>797</v>
       </c>
-    </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B297">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>798</v>
       </c>
-    </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B298">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>799</v>
       </c>
-    </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B299">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>800</v>
       </c>
-    </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B300">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>801</v>
       </c>
-    </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B301">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>802</v>
       </c>
-    </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B302">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>803</v>
       </c>
-    </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B303">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>804</v>
       </c>
-    </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B304">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>805</v>
       </c>
-    </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B305">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B306">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B307">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B308">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>809</v>
       </c>
-    </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B309">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>810</v>
       </c>
-    </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B310">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>811</v>
       </c>
-    </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B311">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>812</v>
       </c>
-    </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B312">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>813</v>
       </c>
-    </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B313">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>814</v>
       </c>
-    </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B314">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>815</v>
       </c>
-    </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B315">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>816</v>
       </c>
-    </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B316">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>817</v>
       </c>
-    </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B317">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>818</v>
       </c>
-    </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B318">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>819</v>
       </c>
-    </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B319">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>820</v>
       </c>
-    </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B320">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>821</v>
       </c>
-    </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B321">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>822</v>
       </c>
-    </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B322">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>823</v>
       </c>
-    </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B323">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>824</v>
       </c>
-    </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B324">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>825</v>
       </c>
-    </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B325">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>826</v>
       </c>
-    </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B326">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>827</v>
       </c>
-    </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B327">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>828</v>
+      </c>
+      <c r="B328">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correção de erros, agora sim ambas tabelas estão preenchidas
</commit_message>
<xml_diff>
--- a/havaiana.xlsx
+++ b/havaiana.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilh\OneDrive - Insper - Institudo de Ensino e Pesquisa\2° Semestre\Ciência dos Dados\Projeto1-Ciedados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="116" documentId="6_{1388BAEF-BB38-4AB5-96FF-C5BA3AC9A653}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CBFC8002-02FB-4D0D-88EB-A94A3EC21982}"/>
+  <xr:revisionPtr revIDLastSave="149" documentId="6_{1388BAEF-BB38-4AB5-96FF-C5BA3AC9A653}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{68E3FE3A-A0F4-4B78-8EED-422BF89A66BA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -2716,12 +2716,13 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -3063,8 +3064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B501"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B501" sqref="B501"/>
+    <sheetView tabSelected="1" topLeftCell="A274" workbookViewId="0">
+      <selection activeCell="B300" sqref="B300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5245,640 +5246,1024 @@
       <c r="A272" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B272">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B273">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B274">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B275">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B276">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B277">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B278">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B279">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B280">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B281">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B282">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B283">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B284">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B285">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B286">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B287">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B288">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B289">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B290">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B291">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B292">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B293">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B294">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B295">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B296">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B297">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B298">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B299">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B300" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B301" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B302" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B303" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B304" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B305" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B306" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B307" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B308" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B309" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B310" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B311" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B312" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B313" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B314" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B315" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B316" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B317" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B318" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B319" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B320" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B321" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B322" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B323" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B324" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B325" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B326" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B327" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B328" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B329" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B330" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B331" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B332" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B333" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B334" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B335" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B336" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B337" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B338" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B339" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B340" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B341" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B342" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B343" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B344" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B345" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B346" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B347" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B348" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B349" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B350" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B351" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B352" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B353" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B354" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B355" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B356" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B357" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B358" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B359" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B360" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B361" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B362" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B363" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B364" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B365" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B366" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B367" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B368" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B369" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B370" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B371" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B372" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B373" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B374" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B375" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B376" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B377" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B378" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B379" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B380" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B381" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B382" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B383" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>383</v>
+      </c>
+      <c r="B384" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>384</v>
       </c>
+      <c r="B385" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>385</v>
       </c>
+      <c r="B386" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>386</v>
       </c>
+      <c r="B387" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>387</v>
       </c>
+      <c r="B388" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>388</v>
       </c>
+      <c r="B389" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>389</v>
       </c>
+      <c r="B390" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>390</v>
       </c>
+      <c r="B391" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>391</v>
       </c>
+      <c r="B392" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>392</v>
       </c>
+      <c r="B393" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>393</v>
       </c>
+      <c r="B394" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>394</v>
       </c>
+      <c r="B395" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>395</v>
       </c>
+      <c r="B396" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>396</v>
       </c>
+      <c r="B397" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>397</v>
       </c>
+      <c r="B398" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>398</v>
+      </c>
+      <c r="B399" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.25">
@@ -6709,7 +7094,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B328"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A303" workbookViewId="0">
+    <sheetView topLeftCell="A303" workbookViewId="0">
       <selection activeCell="B201" sqref="B201:B328"/>
     </sheetView>
   </sheetViews>

</xml_diff>